<commit_message>
update "tag_1, tag_2" in multiples
</commit_message>
<xml_diff>
--- a/data/CLEAN_LISTS.xlsx
+++ b/data/CLEAN_LISTS.xlsx
@@ -39,10 +39,10 @@
     <t>entity_2</t>
   </si>
   <si>
-    <t>tag_1</t>
-  </si>
-  <si>
-    <t>tag_2</t>
+    <t>type_1</t>
+  </si>
+  <si>
+    <t>type_2</t>
   </si>
   <si>
     <t>context</t>

</xml_diff>